<commit_message>
Replica files as ordered, GNURadio blocks
</commit_message>
<xml_diff>
--- a/Ground Station/Link Budgets.xlsx
+++ b/Ground Station/Link Budgets.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22624"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="0" windowWidth="24740" windowHeight="15620" activeTab="1"/>
+    <workbookView xWindow="4860" yWindow="0" windowWidth="24740" windowHeight="15620"/>
   </bookViews>
   <sheets>
     <sheet name="Sprite Link Budget" sheetId="1" r:id="rId1"/>
@@ -16,8 +16,8 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="P - Personal View" guid="{56B56577-359B-4FEF-8511-5634C3B3AD8C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1017" windowHeight="629" activeSheetId="1"/>
     <customWorkbookView name="Justin Atchison - Personal View" guid="{DF438D20-ED32-4502-BBF3-1338727B4A2A}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1011" windowHeight="646" activeSheetId="1"/>
-    <customWorkbookView name="P - Personal View" guid="{56B56577-359B-4FEF-8511-5634C3B3AD8C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1017" windowHeight="629" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -1289,8 +1289,8 @@
   </sheetPr>
   <dimension ref="B1:P93"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1774,11 +1774,11 @@
       </c>
       <c r="C26" s="68">
         <f>10^(E26/10)</f>
-        <v>50.118723362727238</v>
+        <v>10</v>
       </c>
       <c r="D26" s="95"/>
       <c r="E26" s="99">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F26" s="96" t="s">
         <v>2</v>
@@ -1826,11 +1826,11 @@
       </c>
       <c r="C28" s="108">
         <f>10^(E28/10)</f>
-        <v>3.1622776601683795</v>
+        <v>25.118864315095799</v>
       </c>
       <c r="D28" s="109"/>
       <c r="E28" s="110">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F28" s="106" t="s">
         <v>2</v>
@@ -1900,7 +1900,7 @@
       </c>
       <c r="C31" s="71">
         <f>$C$7*C27*(C30*1000)*C28</f>
-        <v>6.3306994202824191E-16</v>
+        <v>5.0286532950829657E-15</v>
       </c>
       <c r="D31" s="94" t="s">
         <v>7</v>
@@ -2139,14 +2139,14 @@
       </c>
       <c r="C42" s="77">
         <f>$C$34*$C$23*C29*$C$24*C26*C33</f>
-        <v>1.2774089166453613E-15</v>
+        <v>2.5487658721877117E-16</v>
       </c>
       <c r="D42" s="78" t="s">
         <v>7</v>
       </c>
       <c r="E42" s="79">
         <f>$E$34+$E$23+$E$24+E29+E26+E33</f>
-        <v>-148.952503286352</v>
+        <v>-155.952503286352</v>
       </c>
       <c r="F42" s="78" t="s">
         <v>6</v>
@@ -2165,12 +2165,12 @@
       </c>
       <c r="C43" s="80">
         <f>C42/C31</f>
-        <v>2.017800612287441</v>
+        <v>5.0684859794965453E-2</v>
       </c>
       <c r="D43" s="78"/>
       <c r="E43" s="79">
         <f>10*LOG10(C43)</f>
-        <v>3.0487824948191315</v>
+        <v>-12.951217505180868</v>
       </c>
       <c r="F43" s="78" t="s">
         <v>2</v>
@@ -2189,12 +2189,12 @@
       </c>
       <c r="C44" s="81">
         <f>C42*C40/C31</f>
-        <v>1033.1139134911698</v>
+        <v>25.950648215022312</v>
       </c>
       <c r="D44" s="78"/>
       <c r="E44" s="79">
         <f>10*LOG10(C44)</f>
-        <v>30.141482104577442</v>
+        <v>14.141482104577438</v>
       </c>
       <c r="F44" s="82" t="s">
         <v>2</v>
@@ -2236,12 +2236,12 @@
       </c>
       <c r="C46" s="84">
         <f>C44-C45</f>
-        <v>1023.1139134911698</v>
+        <v>15.950648215022312</v>
       </c>
       <c r="D46" s="85"/>
       <c r="E46" s="86">
         <f>E44-10</f>
-        <v>20.141482104577442</v>
+        <v>4.1414821045774382</v>
       </c>
       <c r="F46" s="87" t="s">
         <v>2</v>
@@ -2924,13 +2924,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DF438D20-ED32-4502-BBF3-1338727B4A2A}" showRuler="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <customSheetView guid="{56B56577-359B-4FEF-8511-5634C3B3AD8C}" showRuler="0">
+      <selection activeCell="L18" sqref="L18"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{56B56577-359B-4FEF-8511-5634C3B3AD8C}" showRuler="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <customSheetView guid="{DF438D20-ED32-4502-BBF3-1338727B4A2A}" showRuler="0">
+      <selection activeCell="D24" sqref="D24"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
@@ -2969,7 +2969,7 @@
   </sheetPr>
   <dimension ref="B1:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>

</xml_diff>